<commit_message>
add web page on Web2, and message for it
</commit_message>
<xml_diff>
--- a/AutoManagedNodes.xlsx
+++ b/AutoManagedNodes.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jplaberge/Documents/workspace.2016-b/krr.git/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="24260" windowHeight="15120" tabRatio="500"/>
+    <workbookView xWindow="840" yWindow="480" windowWidth="24260" windowHeight="15120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -254,6 +262,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -581,13 +594,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -598,7 +611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -609,7 +622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -620,7 +633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -631,7 +644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -642,7 +655,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -653,7 +666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -664,7 +677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -675,7 +688,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -686,7 +699,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -697,7 +710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -708,7 +721,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -719,7 +732,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -730,7 +743,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -741,7 +754,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -752,7 +765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -763,7 +776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -774,7 +787,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -785,7 +798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -796,7 +809,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -807,7 +820,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -818,7 +831,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -832,10 +845,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>